<commit_message>
almost nailed driver selection
</commit_message>
<xml_diff>
--- a/modules/data/resources/accounts.xlsx
+++ b/modules/data/resources/accounts.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -736,6 +736,76 @@
         <v>95876893</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Geanne.S83@gmail.com</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>63014224</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>B_Mons32@yahoo.com</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>32992576</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>SaadetB29@kpnmail.nl</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>56928796</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Ilian_B@gmail.com</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>93898430</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>L.Lagendijk@live.com</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>38370214</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Sippie_O@hotmail.com</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>44864502</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>S.Hameleers26@kpnmail.nl</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>16331942</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
trying to fix dataframe bug in create account ln 108
</commit_message>
<xml_diff>
--- a/modules/data/resources/accounts.xlsx
+++ b/modules/data/resources/accounts.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -806,6 +806,96 @@
         <v>16331942</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Shaun_M70@gmail.com</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>47144029</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>J.Biesheuvel56@yahoo.com</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>20181690</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Mohsin.S@yahoo.com</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>26571302</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>J_Vente@hotmail.com</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>40987142</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Pia_A@yahoo.com</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>58075440</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Tooske_W@xs4all.nl</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>68073468</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Badia.G81@hotmail.com</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>79961625</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ChanineG@xs4all.nl</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>89579070</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Dila.Stein@kpnmail.nl</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>17167209</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
wait for element load
</commit_message>
<xml_diff>
--- a/modules/data/resources/accounts.xlsx
+++ b/modules/data/resources/accounts.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -896,6 +896,16 @@
         <v>17167209</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Jeremi.Beld@live.com</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>62267877</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>